<commit_message>
FINAL COMMIT - INSIGHTS AND RECOMMENDATIONS
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -170,7 +170,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -261,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -292,14 +292,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="72">
     <dxf>
-      <numFmt numFmtId="171" formatCode="0.0000000000"/>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -310,6 +320,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -324,30 +337,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -388,106 +377,22 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -622,10 +527,64 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -795,6 +754,54 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
@@ -1672,14 +1679,14 @@
   <tableColumns count="10">
     <tableColumn id="21" uniqueName="21" name="Campaign Name" queryTableFieldId="1" dataDxfId="71"/>
     <tableColumn id="22" uniqueName="22" name="Date" queryTableFieldId="2" dataDxfId="70"/>
-    <tableColumn id="23" uniqueName="23" name="Spend [USD]" queryTableFieldId="3" dataDxfId="21"/>
-    <tableColumn id="24" uniqueName="24" name="# of Impressions" queryTableFieldId="4" dataDxfId="20"/>
-    <tableColumn id="25" uniqueName="25" name="Reach" queryTableFieldId="5" dataDxfId="19"/>
-    <tableColumn id="26" uniqueName="26" name="# of Website Clicks" queryTableFieldId="6" dataDxfId="18"/>
-    <tableColumn id="27" uniqueName="27" name="# of Searches" queryTableFieldId="7" dataDxfId="17"/>
-    <tableColumn id="28" uniqueName="28" name="# of View Content" queryTableFieldId="8" dataDxfId="16"/>
-    <tableColumn id="29" uniqueName="29" name="# of Add to Cart" queryTableFieldId="9" dataDxfId="15"/>
-    <tableColumn id="30" uniqueName="30" name="# of Purchase" queryTableFieldId="10" dataDxfId="14"/>
+    <tableColumn id="23" uniqueName="23" name="Spend [USD]" queryTableFieldId="3" dataDxfId="69"/>
+    <tableColumn id="24" uniqueName="24" name="# of Impressions" queryTableFieldId="4" dataDxfId="68"/>
+    <tableColumn id="25" uniqueName="25" name="Reach" queryTableFieldId="5" dataDxfId="67"/>
+    <tableColumn id="26" uniqueName="26" name="# of Website Clicks" queryTableFieldId="6" dataDxfId="66"/>
+    <tableColumn id="27" uniqueName="27" name="# of Searches" queryTableFieldId="7" dataDxfId="65"/>
+    <tableColumn id="28" uniqueName="28" name="# of View Content" queryTableFieldId="8" dataDxfId="64"/>
+    <tableColumn id="29" uniqueName="29" name="# of Add to Cart" queryTableFieldId="9" dataDxfId="63"/>
+    <tableColumn id="30" uniqueName="30" name="# of Purchase" queryTableFieldId="10" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1689,20 +1696,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table18" displayName="Table18" ref="A18:F26" totalsRowShown="0">
   <autoFilter ref="A18:F26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Feature" dataDxfId="5"/>
-    <tableColumn id="2" name="Avg. Test Group" dataDxfId="4">
+    <tableColumn id="1" name="Feature" dataDxfId="7"/>
+    <tableColumn id="2" name="Avg. Test Group" dataDxfId="6">
       <calculatedColumnFormula>AVERAGE(test_group[Spend '[USD']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Avg. Control Group" dataDxfId="3">
+    <tableColumn id="3" name="Avg. Control Group" dataDxfId="5">
       <calculatedColumnFormula>AVERAGE(control_group[Spend '[USD']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="P-Value" dataDxfId="0">
+    <tableColumn id="4" name="P-Value" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.T.TEST(test_group[Spend '[USD']], control_group[Spend '[USD']],2,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Significant (p &lt; 0.05)?" dataDxfId="2">
+    <tableColumn id="5" name="Significant (p &lt; 0.05)?" dataDxfId="3">
       <calculatedColumnFormula>IF(Table18[[#This Row],[P-Value]]&lt;0.05,"YES","NO")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Better Campaign" dataDxfId="1">
+    <tableColumn id="6" name="Better Campaign" dataDxfId="2">
       <calculatedColumnFormula>IF(Table18[[#This Row],[Avg. Test Group]]&gt;Table18[[#This Row],[Avg. Control Group]],"TEST","CONTROL")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1715,49 +1722,49 @@
   <autoFilter ref="B34:J40"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Value / Feature"/>
-    <tableColumn id="2" name="Spend [USD]" dataDxfId="45">
+    <tableColumn id="2" name="Spend [USD]" dataDxfId="61">
       <calculatedColumnFormula>MIN(test_group[Spend '[USD']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="# of Impressions" dataDxfId="44">
+    <tableColumn id="3" name="# of Impressions" dataDxfId="60">
       <calculatedColumnFormula>MIN(test_group['# of Impressions])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Reach" dataDxfId="43"/>
-    <tableColumn id="5" name="# of Website Clicks" dataDxfId="42"/>
-    <tableColumn id="6" name="# of Searches" dataDxfId="41"/>
-    <tableColumn id="7" name="# of View Content" dataDxfId="40"/>
-    <tableColumn id="8" name="# of Add to Cart" dataDxfId="39"/>
-    <tableColumn id="9" name="# of Purchase" dataDxfId="38"/>
+    <tableColumn id="4" name="Reach" dataDxfId="59"/>
+    <tableColumn id="5" name="# of Website Clicks" dataDxfId="58"/>
+    <tableColumn id="6" name="# of Searches" dataDxfId="57"/>
+    <tableColumn id="7" name="# of View Content" dataDxfId="56"/>
+    <tableColumn id="8" name="# of Add to Cart" dataDxfId="55"/>
+    <tableColumn id="9" name="# of Purchase" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="test_group_zscore" displayName="test_group_zscore" ref="C43:J73" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="test_group_zscore" displayName="test_group_zscore" ref="C43:J73" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="C43:J73"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Spend [USD] Z-score" dataDxfId="67">
+    <tableColumn id="1" name="Spend [USD] Z-score" dataDxfId="51">
       <calculatedColumnFormula>(C2-$C$37)/$C$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="# of Impressions Z-score" dataDxfId="66">
+    <tableColumn id="2" name="# of Impressions Z-score" dataDxfId="50">
       <calculatedColumnFormula>(D2-$D$37)/$D$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Reach Z-score" dataDxfId="65">
+    <tableColumn id="3" name="Reach Z-score" dataDxfId="49">
       <calculatedColumnFormula>(E2-$E$37)/$E$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="# of Website Clicks Z-score" dataDxfId="64">
+    <tableColumn id="4" name="# of Website Clicks Z-score" dataDxfId="48">
       <calculatedColumnFormula>(F2-$F$37)/$F$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="# of Searches Z-score" dataDxfId="63">
+    <tableColumn id="5" name="# of Searches Z-score" dataDxfId="47">
       <calculatedColumnFormula>(G2-$G$37)/$G$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="# of View Content Z-score" dataDxfId="62">
+    <tableColumn id="6" name="# of View Content Z-score" dataDxfId="46">
       <calculatedColumnFormula>(H2-$H$37)/$H$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="# of Add to Cart Z-score" dataDxfId="61">
+    <tableColumn id="7" name="# of Add to Cart Z-score" dataDxfId="45">
       <calculatedColumnFormula>(I2-$I$37)/$I$39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="# of Purchase Z-score" dataDxfId="60">
+    <tableColumn id="8" name="# of Purchase Z-score" dataDxfId="44">
       <calculatedColumnFormula>(J2-$J$37)/$J$39</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1766,14 +1773,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="L43:O51" totalsRowShown="0" headerRowDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="L43:O51" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="L43:O51"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Feature / Value"/>
-    <tableColumn id="2" name="Min Z-score" dataDxfId="13">
+    <tableColumn id="2" name="Min Z-score" dataDxfId="42">
       <calculatedColumnFormula>MIN(test_group_zscore[Spend '[USD'] Z-score])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Max Z-score" dataDxfId="12">
+    <tableColumn id="3" name="Max Z-score" dataDxfId="41">
       <calculatedColumnFormula>MAX(test_group_zscore[Spend '[USD'] Z-score])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Outliers Detected"/>
@@ -1786,16 +1793,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="control_group" displayName="control_group" ref="A1:J31" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:J31"/>
   <tableColumns count="10">
-    <tableColumn id="21" uniqueName="21" name="Campaign Name" queryTableFieldId="1" dataDxfId="58"/>
-    <tableColumn id="22" uniqueName="22" name="Date" queryTableFieldId="2" dataDxfId="57"/>
-    <tableColumn id="23" uniqueName="23" name="Spend [USD]" queryTableFieldId="3" dataDxfId="29"/>
-    <tableColumn id="24" uniqueName="24" name="# of Impressions" queryTableFieldId="4" dataDxfId="28"/>
-    <tableColumn id="25" uniqueName="25" name="Reach" queryTableFieldId="5" dataDxfId="27"/>
-    <tableColumn id="26" uniqueName="26" name="# of Website Clicks" queryTableFieldId="6" dataDxfId="26"/>
-    <tableColumn id="27" uniqueName="27" name="# of Searches" queryTableFieldId="7" dataDxfId="25"/>
-    <tableColumn id="28" uniqueName="28" name="# of View Content" queryTableFieldId="8" dataDxfId="24"/>
-    <tableColumn id="29" uniqueName="29" name="# of Add to Cart" queryTableFieldId="9" dataDxfId="23"/>
-    <tableColumn id="30" uniqueName="30" name="# of Purchase" queryTableFieldId="10" dataDxfId="22"/>
+    <tableColumn id="21" uniqueName="21" name="Campaign Name" queryTableFieldId="1" dataDxfId="40"/>
+    <tableColumn id="22" uniqueName="22" name="Date" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn id="23" uniqueName="23" name="Spend [USD]" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="24" uniqueName="24" name="# of Impressions" queryTableFieldId="4" dataDxfId="37"/>
+    <tableColumn id="25" uniqueName="25" name="Reach" queryTableFieldId="5" dataDxfId="36"/>
+    <tableColumn id="26" uniqueName="26" name="# of Website Clicks" queryTableFieldId="6" dataDxfId="35"/>
+    <tableColumn id="27" uniqueName="27" name="# of Searches" queryTableFieldId="7" dataDxfId="34"/>
+    <tableColumn id="28" uniqueName="28" name="# of View Content" queryTableFieldId="8" dataDxfId="33"/>
+    <tableColumn id="29" uniqueName="29" name="# of Add to Cart" queryTableFieldId="9" dataDxfId="32"/>
+    <tableColumn id="30" uniqueName="30" name="# of Purchase" queryTableFieldId="10" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1806,51 +1813,51 @@
   <autoFilter ref="B33:J39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Value / Feature"/>
-    <tableColumn id="2" name="Spend [USD]" dataDxfId="37">
+    <tableColumn id="2" name="Spend [USD]" dataDxfId="30">
       <calculatedColumnFormula>MIN(control_group[Spend '[USD']])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="# of Impressions" dataDxfId="36">
+    <tableColumn id="3" name="# of Impressions" dataDxfId="29">
       <calculatedColumnFormula>MIN(control_group['# of Impressions])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Reach" dataDxfId="35">
+    <tableColumn id="4" name="Reach" dataDxfId="28">
       <calculatedColumnFormula>MIN(control_group[Reach])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="# of Website Clicks" dataDxfId="34"/>
-    <tableColumn id="6" name="# of Searches" dataDxfId="33"/>
-    <tableColumn id="7" name="# of View Content" dataDxfId="32"/>
-    <tableColumn id="8" name="# of Add to Cart" dataDxfId="31"/>
-    <tableColumn id="9" name="# of Purchase" dataDxfId="30"/>
+    <tableColumn id="5" name="# of Website Clicks" dataDxfId="27"/>
+    <tableColumn id="6" name="# of Searches" dataDxfId="26"/>
+    <tableColumn id="7" name="# of View Content" dataDxfId="25"/>
+    <tableColumn id="8" name="# of Add to Cart" dataDxfId="24"/>
+    <tableColumn id="9" name="# of Purchase" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="C41:J71" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="C41:J71" totalsRowShown="0" dataDxfId="22">
   <autoFilter ref="C41:J71"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Spend [USD] Z-score" dataDxfId="55">
+    <tableColumn id="1" name="Spend [USD] Z-score" dataDxfId="21">
       <calculatedColumnFormula>(C2-$C$36)/$C$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="# of Impressions Z-score" dataDxfId="54">
+    <tableColumn id="2" name="# of Impressions Z-score" dataDxfId="20">
       <calculatedColumnFormula>(D2-$D$36)/$D$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Reach Z-score" dataDxfId="53">
+    <tableColumn id="3" name="Reach Z-score" dataDxfId="19">
       <calculatedColumnFormula>(E2-$E$36)/$E$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="# of Website Clicks Z-score" dataDxfId="52">
+    <tableColumn id="4" name="# of Website Clicks Z-score" dataDxfId="18">
       <calculatedColumnFormula>(F2-$F$36)/$F$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="# of Searches Z-score" dataDxfId="51">
+    <tableColumn id="5" name="# of Searches Z-score" dataDxfId="17">
       <calculatedColumnFormula>(G2-$G$36)/$G$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="# of View Content Z-score" dataDxfId="50">
+    <tableColumn id="6" name="# of View Content Z-score" dataDxfId="16">
       <calculatedColumnFormula>(H2-$H$36)/$H$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="# of Add to Cart Z-score" dataDxfId="49">
+    <tableColumn id="7" name="# of Add to Cart Z-score" dataDxfId="15">
       <calculatedColumnFormula>(I2-$I$36)/$I$38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="# of Purchase Z-score" dataDxfId="48">
+    <tableColumn id="8" name="# of Purchase Z-score" dataDxfId="14">
       <calculatedColumnFormula>(J2-$J$36)/$J$38</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1863,10 +1870,10 @@
   <autoFilter ref="L41:O49"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Feature / Value"/>
-    <tableColumn id="2" name="Min Z-score" dataDxfId="47">
+    <tableColumn id="2" name="Min Z-score" dataDxfId="13">
       <calculatedColumnFormula>MIN(Table6[Spend '[USD'] Z-score])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Max Z-score" dataDxfId="46">
+    <tableColumn id="3" name="Max Z-score" dataDxfId="12">
       <calculatedColumnFormula>MAX(Table6[Spend '[USD'] Z-score])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Outliers Detected"/>
@@ -1876,16 +1883,16 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="A4:E12" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="A4:E12" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A4:E12"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Feature" dataDxfId="11"/>
-    <tableColumn id="2" name="Test Var" dataDxfId="10"/>
+    <tableColumn id="1" name="Feature" dataDxfId="10"/>
+    <tableColumn id="2" name="Test Var" dataDxfId="9"/>
     <tableColumn id="3" name="Control Var" dataDxfId="8"/>
-    <tableColumn id="4" name="Ratio (larger/smaller)" dataDxfId="7">
+    <tableColumn id="4" name="Ratio (larger/smaller)" dataDxfId="1">
       <calculatedColumnFormula>Table17[[#This Row],[Control Var]]/Table17[[#This Row],[Test Var]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Type" dataDxfId="6">
+    <tableColumn id="5" name="Type" dataDxfId="0">
       <calculatedColumnFormula>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7088,7 +7095,7 @@
   <dimension ref="A3:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,7 +7155,7 @@
         <f>Table17[[#This Row],[Control Var]]/Table17[[#This Row],[Test Var]]</f>
         <v>1.109813782723279</v>
       </c>
-      <c r="E5" s="11" t="str">
+      <c r="E5" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>equal var</v>
       </c>
@@ -7173,7 +7180,7 @@
         <f>Table17[[#This Row],[Test Var]]/Table17[[#This Row],[Control Var]]</f>
         <v>2.2717070041154854</v>
       </c>
-      <c r="E6" s="11" t="str">
+      <c r="E6" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>unequal var</v>
       </c>
@@ -7198,7 +7205,7 @@
         <f>Table17[[#This Row],[Test Var]]/Table17[[#This Row],[Control Var]]</f>
         <v>1.8017584946956535</v>
       </c>
-      <c r="E7" s="11" t="str">
+      <c r="E7" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>equal var</v>
       </c>
@@ -7223,7 +7230,7 @@
         <f>Table17[[#This Row],[Control Var]]/Table17[[#This Row],[Test Var]]</f>
         <v>1.0214610142361327</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>equal var</v>
       </c>
@@ -7248,7 +7255,7 @@
         <f>Table17[[#This Row],[Control Var]]/Table17[[#This Row],[Test Var]]</f>
         <v>3.1234764031064541</v>
       </c>
-      <c r="E9" s="11" t="str">
+      <c r="E9" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>unequal var</v>
       </c>
@@ -7269,7 +7276,7 @@
         <f>Table17[[#This Row],[Control Var]]/Table17[[#This Row],[Test Var]]</f>
         <v>1.6342217619642507</v>
       </c>
-      <c r="E10" s="11" t="str">
+      <c r="E10" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>equal var</v>
       </c>
@@ -7290,7 +7297,7 @@
         <f>Table17[[#This Row],[Control Var]]/Table17[[#This Row],[Test Var]]</f>
         <v>1.3268001209108078</v>
       </c>
-      <c r="E11" s="11" t="str">
+      <c r="E11" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>equal var</v>
       </c>
@@ -7311,7 +7318,7 @@
         <f>Table17[[#This Row],[Test Var]]/Table17[[#This Row],[Control Var]]</f>
         <v>1.3474835534863083</v>
       </c>
-      <c r="E12" s="11" t="str">
+      <c r="E12" s="19" t="str">
         <f>IF(Table17[[#This Row],[Ratio (larger/smaller)]]&lt;2,"equal var","unequal var")</f>
         <v>equal var</v>
       </c>
@@ -7544,10 +7551,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>